<commit_message>
EF Core finished. All working.
</commit_message>
<xml_diff>
--- a/Time recording log week 1.xlsx
+++ b/Time recording log week 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristen\source\repos\Kodusedtööd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE76DE1-776C-4BB4-80E0-37D2BAC6AC76}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DA292E-93A1-47A8-9D37-2F2438500315}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="564" windowWidth="22680" windowHeight="11796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Vahetasin oma lauaarvuti CPU jahutit ja lisasin ka sellega kaasneva system fani</t>
   </si>
   <si>
-    <t>html</t>
-  </si>
-  <si>
     <t>06.02.2020</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>EF Core 6 vea fiximine</t>
+  </si>
+  <si>
+    <t>EF Core valmis</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1362,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,7 +1519,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="8">
         <v>0.33333333333333331</v>
@@ -1532,10 +1532,10 @@
         <v>150</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
@@ -1545,7 +1545,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="8">
         <v>0.4375</v>
@@ -1558,10 +1558,10 @@
         <v>80</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1571,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="8">
         <v>0.4375</v>
@@ -1586,10 +1586,10 @@
         <v>300</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -1599,7 +1599,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8">
         <v>0.70833333333333337</v>
@@ -1612,10 +1612,10 @@
         <v>60</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1625,7 +1625,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="8">
         <v>0.41319444444444442</v>
@@ -1638,10 +1638,10 @@
         <v>40</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
@@ -1650,15 +1650,25 @@
       <c r="A13" s="9">
         <v>8</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.92013888888888884</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6">
+        <v>215</v>
+      </c>
       <c r="G13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="31"/>
+        <v>38</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>46</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -1671,9 +1681,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="G14" s="6"/>
       <c r="H14" s="31"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1730,7 +1738,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="35">
         <f>SUM(F6:F17)</f>
-        <v>820</v>
+        <v>1035</v>
       </c>
       <c r="G18" s="36"/>
       <c r="H18" s="36"/>

</xml_diff>

<commit_message>
2. kodutöö esimene commit
</commit_message>
<xml_diff>
--- a/Time recording log week 1.xlsx
+++ b/Time recording log week 1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristen\source\repos\Kodusedtööd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DA292E-93A1-47A8-9D37-2F2438500315}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA6BCDC-DABB-4856-BAC5-EEAE0164FEC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="564" windowWidth="22680" windowHeight="11796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
     <sheet name="Nädal 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Nädal 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -173,6 +174,18 @@
   </si>
   <si>
     <t>EF Core valmis</t>
+  </si>
+  <si>
+    <t>11.02.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milleks on õppejõud? </t>
+  </si>
+  <si>
+    <t>PodCast</t>
+  </si>
+  <si>
+    <t>Algorütm 2</t>
   </si>
 </sst>
 </file>
@@ -998,22 +1011,22 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="53.44140625" customWidth="1"/>
-    <col min="9" max="9" width="3.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" customWidth="1"/>
+    <col min="8" max="8" width="53.453125" customWidth="1"/>
+    <col min="9" max="9" width="3.54296875" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1040,7 @@
       <c r="I2" s="45"/>
       <c r="J2" s="46"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="47"/>
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
@@ -1039,7 +1052,7 @@
       <c r="I3" s="48"/>
       <c r="J3" s="49"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="56" t="s">
         <v>1</v>
       </c>
@@ -1059,7 +1072,7 @@
       <c r="I4" s="51"/>
       <c r="J4" s="52"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="53"/>
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
@@ -1071,7 +1084,7 @@
       <c r="I5" s="54"/>
       <c r="J5" s="55"/>
     </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
         <v>3</v>
       </c>
@@ -1101,7 +1114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1131,7 +1144,7 @@
       </c>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>2</v>
       </c>
@@ -1161,7 +1174,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>3</v>
       </c>
@@ -1191,7 +1204,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>4</v>
       </c>
@@ -1219,14 +1232,14 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>5</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>6</v>
       </c>
@@ -1240,7 +1253,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>7</v>
       </c>
@@ -1254,7 +1267,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -1268,7 +1281,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>9</v>
       </c>
@@ -1282,7 +1295,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>10</v>
       </c>
@@ -1296,7 +1309,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>11</v>
       </c>
@@ -1310,7 +1323,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -1324,7 +1337,7 @@
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="41" t="s">
         <v>11</v>
       </c>
@@ -1361,18 +1374,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9963A056-09C2-4F28-B447-B38BEDB41D3D}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1399,7 @@
       <c r="I1" s="45"/>
       <c r="J1" s="46"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="47"/>
       <c r="B2" s="58"/>
       <c r="C2" s="58"/>
@@ -1398,7 +1411,7 @@
       <c r="I2" s="58"/>
       <c r="J2" s="49"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="56" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1431,7 @@
       <c r="I3" s="51"/>
       <c r="J3" s="52"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="53"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -1430,7 +1443,7 @@
       <c r="I4" s="59"/>
       <c r="J4" s="55"/>
     </row>
-    <row r="5" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1460,7 +1473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -1486,7 +1499,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="22"/>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9">
         <v>2</v>
       </c>
@@ -1514,7 +1527,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9">
         <v>3</v>
       </c>
@@ -1540,7 +1553,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -1566,7 +1579,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="9">
         <v>5</v>
       </c>
@@ -1594,7 +1607,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="9">
         <v>6</v>
       </c>
@@ -1620,7 +1633,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="9">
         <v>7</v>
       </c>
@@ -1646,7 +1659,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="9">
         <v>8</v>
       </c>
@@ -1672,7 +1685,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="9">
         <v>9</v>
       </c>
@@ -1686,7 +1699,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="9">
         <v>10</v>
       </c>
@@ -1700,7 +1713,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="9">
         <v>11</v>
       </c>
@@ -1714,7 +1727,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="23">
         <v>12</v>
       </c>
@@ -1728,7 +1741,7 @@
       <c r="I17" s="26"/>
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="41" t="s">
         <v>11</v>
       </c>
@@ -1758,4 +1771,329 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1618591-3753-4FE6-8F93-213109760F86}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="8" max="8" width="25.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="47"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="49"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="51">
+        <v>43859</v>
+      </c>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="53"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="55"/>
+    </row>
+    <row r="5" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="17">
+        <v>1</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20">
+        <v>95</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43874</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
+        <v>80</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="9">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="9">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="9">
+        <v>11</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="23">
+        <v>12</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="35">
+        <f>SUM(F6:F17)</f>
+        <v>175</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
"Create complex data model" korras
</commit_message>
<xml_diff>
--- a/Time recording log week 1.xlsx
+++ b/Time recording log week 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristen\source\repos\Kodusedtööd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA6BCDC-DABB-4856-BAC5-EEAE0164FEC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCD69BC-F3D0-4A8C-B126-BCA0F4B5F843}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24585" yWindow="2040" windowWidth="17280" windowHeight="11025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -182,10 +182,16 @@
     <t xml:space="preserve">Milleks on õppejõud? </t>
   </si>
   <si>
-    <t>PodCast</t>
-  </si>
-  <si>
     <t>Algorütm 2</t>
+  </si>
+  <si>
+    <t>Podcast</t>
+  </si>
+  <si>
+    <t>Kodutöö</t>
+  </si>
+  <si>
+    <t>EF Core with MVC</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -691,6 +697,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaallaad" xfId="0" builtinId="0"/>
@@ -1778,7 +1786,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1879,7 +1887,7 @@
       <c r="A6" s="17">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="60" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="19">
@@ -1905,7 +1913,7 @@
       <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="61">
         <v>43874</v>
       </c>
       <c r="C7" s="8">
@@ -1919,10 +1927,10 @@
         <v>80</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>50</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="10"/>
@@ -1931,13 +1939,25 @@
       <c r="A8" s="9">
         <v>3</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="7">
+        <v>43874</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.8125</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.9375</v>
+      </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="6">
+        <v>180</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>52</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1945,13 +1965,25 @@
       <c r="A9" s="9">
         <v>4</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="7">
+        <v>43875</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="31"/>
+      <c r="F9" s="6">
+        <v>165</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>52</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
@@ -1959,13 +1991,25 @@
       <c r="A10" s="9">
         <v>5</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="7">
+        <v>43877</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="31"/>
+      <c r="F10" s="5">
+        <v>250</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>52</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
@@ -2077,7 +2121,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="35">
         <f>SUM(F6:F17)</f>
-        <v>175</v>
+        <v>770</v>
       </c>
       <c r="G18" s="36"/>
       <c r="H18" s="36"/>

</xml_diff>